<commit_message>
Adjusted Index page to have some actual content
</commit_message>
<xml_diff>
--- a/Progress Reports/RyanBury_ProgressReport.xlsx
+++ b/Progress Reports/RyanBury_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Presenting - Creating presentation, revising document</t>
+  </si>
+  <si>
+    <t>Revising - Looking over project, learning some new technologies</t>
+  </si>
+  <si>
+    <t>Learning - Learning how to use the tools that were selected</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,14 +797,26 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="12">
+        <v>42822</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="12">
+        <v>42827</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>

</xml_diff>

<commit_message>
Updated Progress report, added image
</commit_message>
<xml_diff>
--- a/Progress Reports/RyanBury_ProgressReport.xlsx
+++ b/Progress Reports/RyanBury_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>Learning - Learning how to use the tools that were selected</t>
+  </si>
+  <si>
+    <t>Development - Laying framework for website design</t>
+  </si>
+  <si>
+    <t>Development - Getting started!</t>
+  </si>
+  <si>
+    <t>Development - Creating pages</t>
+  </si>
+  <si>
+    <t>Development - Writing Report, fixing pages</t>
+  </si>
+  <si>
+    <t>Development - Beautification of website, fixing bugs</t>
+  </si>
+  <si>
+    <t>Development - Creating pages, adding features</t>
+  </si>
+  <si>
+    <t>Presenting - Demonstration! And last minute fixes before deploying</t>
   </si>
 </sst>
 </file>
@@ -599,7 +620,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,39 +840,81 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="12">
+        <v>42840</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="12">
+        <v>42848</v>
+      </c>
+      <c r="B21" s="6">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="12">
+        <v>42849</v>
+      </c>
+      <c r="B22" s="6">
+        <v>12</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="12">
+        <v>42850</v>
+      </c>
+      <c r="B23" s="6">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="12">
+        <v>42851</v>
+      </c>
+      <c r="B24" s="6">
+        <v>12</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="12">
+        <v>42852</v>
+      </c>
+      <c r="B25" s="6">
+        <v>12</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="12">
+        <v>42853</v>
+      </c>
+      <c r="B26" s="6">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>

</xml_diff>